<commit_message>
started moving things around for better repo structure
</commit_message>
<xml_diff>
--- a/results/ICS_bertopic_combined_topics_Jul-15-2022/hazard_interpretation_v1.xlsx
+++ b/results/ICS_bertopic_combined_topics_Jul-15-2022/hazard_interpretation_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srandrad\smart_nlp\results\ICS_bertopic_combined_topics_Jul-15-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AC052A-CDF7-4BB7-9130-3A3392D02794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC40CD3-0A66-4B4A-9926-E1ACE291BA15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10044" firstSheet="1" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="1" xr2:uid="{1E09127A-9D7A-4A65-B2FF-C060090E7D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hazard-focused" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>Hazardous Terrain</t>
   </si>
   <si>
-    <t>Innacurate Mapping</t>
-  </si>
-  <si>
     <t>Ecological Resources</t>
   </si>
   <si>
@@ -278,6 +275,9 @@
   </si>
   <si>
     <t>open, reopen, lift, area, trail, facility, park, campground, impact, access, narrow, rough, operations, line, integrety, operation, preparation, burnout, burn, prep, jumped, crossed, windy, fire</t>
+  </si>
+  <si>
+    <t>Inaccurate Mapping</t>
   </si>
 </sst>
 </file>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E799D7D2-7755-4A40-8FAC-FBB6E32500C5}">
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -743,16 +743,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N2" t="s">
         <v>14</v>
       </c>
       <c r="P2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>15</v>
@@ -760,13 +760,13 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>16</v>
@@ -774,258 +774,258 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="T5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="P16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="P20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>